<commit_message>
comment out export_M2_records button
</commit_message>
<xml_diff>
--- a/ConfigFile/M2/test.xlsx
+++ b/ConfigFile/M2/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>编号</t>
   </si>
@@ -24,6 +24,18 @@
   </si>
   <si>
     <t>M2 IP</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>左线</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10.1.2.2</t>
   </si>
 </sst>
 </file>
@@ -68,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -88,6 +100,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
1.add prompt info after way and DK updated;2.add auto_export after ST created;3.no need to fire the browser if only update way and DK;4.add auto_export data after removea row
</commit_message>
<xml_diff>
--- a/ConfigFile/M2/test.xlsx
+++ b/ConfigFile/M2/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>编号</t>
   </si>
@@ -24,18 +24,6 @@
   </si>
   <si>
     <t>M2 IP</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>左线</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>10.1.2.2</t>
   </si>
 </sst>
 </file>
@@ -80,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -100,20 +88,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>